<commit_message>
re-envisioned loading sheet tab loading logic. fixed #704, #708
</commit_message>
<xml_diff>
--- a/src/test/resources/custom.xlsx
+++ b/src/test/resources/custom.xlsx
@@ -5,39 +5,20 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="596" firstSheet="0" activeTab="2"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="539" firstSheet="0" activeTab="0"/>
   </bookViews>
   <sheets>
-    <sheet name="Loader" sheetId="1" state="visible" r:id="rId2"/>
-    <sheet name="Metadata" sheetId="2" state="visible" r:id="rId3"/>
-    <sheet name="Categories" sheetId="3" state="visible" r:id="rId4"/>
-    <sheet name="Products" sheetId="4" state="visible" r:id="rId5"/>
-    <sheet name="Product Categories" sheetId="5" state="visible" r:id="rId6"/>
+    <sheet name="Sheet4" sheetId="1" state="visible" r:id="rId2"/>
+    <sheet name="Categories" sheetId="2" state="visible" r:id="rId3"/>
+    <sheet name="Products" sheetId="3" state="visible" r:id="rId4"/>
+    <sheet name="Product Categories" sheetId="4" state="visible" r:id="rId5"/>
   </sheets>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.0001"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="169" uniqueCount="97">
-  <si>
-    <t>Sheet Name</t>
-  </si>
-  <si>
-    <t>Type</t>
-  </si>
-  <si>
-    <t>Categories</t>
-  </si>
-  <si>
-    <t>Usual</t>
-  </si>
-  <si>
-    <t>Products</t>
-  </si>
-  <si>
-    <t>Product Categories</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="147" uniqueCount="79">
   <si>
     <t>Metadata</t>
   </si>
@@ -69,12 +50,6 @@
     <t>http://xmlns.com/foaf/0.1/</t>
   </si>
   <si>
-    <t>owl:versionIRI</t>
-  </si>
-  <si>
-    <t>http://seman.tc/data/northwind/0.9</t>
-  </si>
-  <si>
     <t>northwind:</t>
   </si>
   <si>
@@ -84,40 +59,10 @@
     <t>http://purl.org/dc/terms/</t>
   </si>
   <si>
-    <t>owl:versionInfo</t>
-  </si>
-  <si>
-    <t>"0.9"^^xsd:float</t>
-  </si>
-  <si>
-    <t>dct:creator</t>
-  </si>
-  <si>
-    <t>North Wind, LLC</t>
-  </si>
-  <si>
-    <t>dct:description</t>
-  </si>
-  <si>
-    <t>This is the "North Wind" Testing Database</t>
-  </si>
-  <si>
-    <t>dct:publisher</t>
-  </si>
-  <si>
-    <t>North Wind, LLC &lt;info@com.northwind&gt;</t>
+    <t>schema:subject</t>
   </si>
   <si>
     <t>rdfs:label</t>
-  </si>
-  <si>
-    <t>"Northwind Corporate Database"^^xsd:string</t>
-  </si>
-  <si>
-    <t>@triple</t>
-  </si>
-  <si>
-    <t>schema:subject</t>
   </si>
   <si>
     <t>http://junk/just-for-fun</t>
@@ -419,57 +364,246 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:B5"/>
+  <dimension ref="A1:D7"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A3" activeCellId="0" sqref="A3"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A7" activeCellId="0" sqref="A7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="23.5748987854251"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="9.4251012145749"/>
-    <col collapsed="false" hidden="false" max="1025" min="3" style="0" width="8.53441295546559"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="9.06882591093117"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="19.5465587044534"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="10.2834008097166"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="31.2348178137652"/>
+    <col collapsed="false" hidden="false" max="1025" min="5" style="0" width="9.1417004048583"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="0" t="s">
+      <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="0" t="s">
-        <v>1</v>
+      <c r="B1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="2"/>
+      <c r="D1" s="1" t="s">
+        <v>2</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="0" t="s">
-        <v>2</v>
-      </c>
-      <c r="B2" s="0" t="s">
+      <c r="A2" s="1"/>
+      <c r="B2" s="1" t="s">
         <v>3</v>
       </c>
+      <c r="C2" s="2"/>
+      <c r="D2" s="1" t="s">
+        <v>4</v>
+      </c>
     </row>
     <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="0" t="s">
+      <c r="A3" s="1"/>
+      <c r="B3" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="C3" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="D3" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4" s="1"/>
+      <c r="B4" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="C4" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="D4" s="1" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="5" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A5" s="1"/>
+      <c r="B5" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="C5" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="D5" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="B3" s="0" t="s">
-        <v>3</v>
+    </row>
+    <row r="6" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A6" s="1"/>
+      <c r="B6" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="C6" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="D6" s="1" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="7" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A7" s="1"/>
+      <c r="B7" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="C7" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="D7" s="1" t="s">
+        <v>15</v>
+      </c>
+    </row>
+  </sheetData>
+  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
+  <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
+  <pageSetup paperSize="1" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <headerFooter differentFirst="false" differentOddEven="false">
+    <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
+    <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
+  </headerFooter>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <sheetPr filterMode="false">
+    <pageSetUpPr fitToPage="false"/>
+  </sheetPr>
+  <dimension ref="A1:D10"/>
+  <sheetViews>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="B10" activeCellId="0" sqref="B10"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="13.8"/>
+  <cols>
+    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="8.53441295546559"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="14.1417004048583"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="1" width="34.2834008097166"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="1" width="30.6518218623482"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="1" width="11.3562753036437"/>
+    <col collapsed="false" hidden="false" max="1025" min="6" style="1" width="8.53441295546559"/>
+  </cols>
+  <sheetData>
+    <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A2" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="D2" s="1" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B3" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="C3" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="D3" s="1" t="s">
+        <v>25</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="0" t="s">
-        <v>5</v>
-      </c>
-      <c r="B4" s="0" t="s">
-        <v>3</v>
+      <c r="B4" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="C4" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="D4" s="1" t="s">
+        <v>28</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="0" t="s">
-        <v>6</v>
-      </c>
-      <c r="B5" s="0" t="s">
-        <v>6</v>
+      <c r="B5" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="C5" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="D5" s="1" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="6" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B6" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="C6" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="D6" s="1" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="7" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B7" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="C7" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="D7" s="1" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="8" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B8" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="C8" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="D8" s="1" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="9" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B9" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="C9" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="D9" s="1" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="10" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B10" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="C10" s="1" t="s">
+        <v>45</v>
       </c>
     </row>
   </sheetData>
@@ -483,313 +617,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <sheetPr filterMode="false">
-    <pageSetUpPr fitToPage="false"/>
-  </sheetPr>
-  <dimension ref="A1:D13"/>
-  <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="86" zoomScaleNormal="86" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A3" activeCellId="0" sqref="A3"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="18.2"/>
-  <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="19.7813765182186"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="14.3967611336032"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="39.6477732793522"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="19.5222672064777"/>
-    <col collapsed="false" hidden="false" max="1025" min="5" style="0" width="9.1417004048583"/>
-  </cols>
-  <sheetData>
-    <row r="1" customFormat="false" ht="18.2" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A1" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="B1" s="2"/>
-      <c r="C1" s="1" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="2" customFormat="false" ht="18.2" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A2" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="B2" s="2"/>
-      <c r="C2" s="1" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="3" customFormat="false" ht="18.2" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A3" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="B3" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="C3" s="1" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="4" customFormat="false" ht="18.2" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A4" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="B4" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="C4" s="1" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="5" customFormat="false" ht="18.2" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A5" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="B5" s="2"/>
-      <c r="C5" s="1" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="6" customFormat="false" ht="18.2" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A6" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="B6" s="2" t="s">
-        <v>18</v>
-      </c>
-      <c r="C6" s="1" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="7" customFormat="false" ht="18.2" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A7" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="B7" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="C7" s="1" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="8" customFormat="false" ht="18.2" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A8" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="B8" s="2"/>
-      <c r="C8" s="1" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="9" customFormat="false" ht="18.2" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A9" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="B9" s="1"/>
-      <c r="C9" s="1" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="10" customFormat="false" ht="18.2" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A10" s="1" t="s">
-        <v>25</v>
-      </c>
-      <c r="B10" s="1"/>
-      <c r="C10" s="1" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="11" customFormat="false" ht="18.2" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A11" s="1" t="s">
-        <v>27</v>
-      </c>
-      <c r="B11" s="1"/>
-      <c r="C11" s="1" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="12" customFormat="false" ht="18.2" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A12" s="1" t="s">
-        <v>29</v>
-      </c>
-      <c r="B12" s="1"/>
-      <c r="C12" s="1" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="13" customFormat="false" ht="18.2" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A13" s="0" t="s">
-        <v>31</v>
-      </c>
-      <c r="B13" s="0" t="s">
-        <v>32</v>
-      </c>
-      <c r="C13" s="0" t="s">
-        <v>29</v>
-      </c>
-      <c r="D13" s="0" t="s">
-        <v>33</v>
-      </c>
-    </row>
-  </sheetData>
-  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
-  <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
-  <pageSetup paperSize="1" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
-  <headerFooter differentFirst="false" differentOddEven="false">
-    <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
-    <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
-  </headerFooter>
-</worksheet>
-</file>
-
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <sheetPr filterMode="false">
-    <pageSetUpPr fitToPage="false"/>
-  </sheetPr>
-  <dimension ref="A1:D10"/>
-  <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B10" activeCellId="0" sqref="B10"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="13.8"/>
-  <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="8.53441295546559"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="14.1417004048583"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="1" width="34.2834008097166"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="1" width="30.6518218623482"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="11.3562753036437"/>
-    <col collapsed="false" hidden="false" max="1025" min="6" style="1" width="8.53441295546559"/>
-  </cols>
-  <sheetData>
-    <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="1" t="s">
-        <v>34</v>
-      </c>
-      <c r="B1" s="1" t="s">
-        <v>35</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>36</v>
-      </c>
-      <c r="D1" s="1" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="1" t="s">
-        <v>37</v>
-      </c>
-      <c r="B2" s="1" t="s">
-        <v>38</v>
-      </c>
-      <c r="C2" s="1" t="s">
-        <v>39</v>
-      </c>
-      <c r="D2" s="1" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B3" s="1" t="s">
-        <v>41</v>
-      </c>
-      <c r="C3" s="1" t="s">
-        <v>42</v>
-      </c>
-      <c r="D3" s="1" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B4" s="1" t="s">
-        <v>44</v>
-      </c>
-      <c r="C4" s="1" t="s">
-        <v>45</v>
-      </c>
-      <c r="D4" s="1" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="5" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B5" s="1" t="s">
-        <v>47</v>
-      </c>
-      <c r="C5" s="1" t="s">
-        <v>48</v>
-      </c>
-      <c r="D5" s="1" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="6" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B6" s="1" t="s">
-        <v>50</v>
-      </c>
-      <c r="C6" s="1" t="s">
-        <v>51</v>
-      </c>
-      <c r="D6" s="1" t="s">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="7" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B7" s="1" t="s">
-        <v>53</v>
-      </c>
-      <c r="C7" s="1" t="s">
-        <v>54</v>
-      </c>
-      <c r="D7" s="1" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="8" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B8" s="1" t="s">
-        <v>56</v>
-      </c>
-      <c r="C8" s="1" t="s">
-        <v>57</v>
-      </c>
-      <c r="D8" s="1" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="9" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B9" s="1" t="s">
-        <v>59</v>
-      </c>
-      <c r="C9" s="1" t="s">
-        <v>60</v>
-      </c>
-      <c r="D9" s="1" t="s">
-        <v>61</v>
-      </c>
-    </row>
-    <row r="10" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B10" s="1" t="s">
-        <v>62</v>
-      </c>
-      <c r="C10" s="1" t="s">
-        <v>63</v>
-      </c>
-    </row>
-  </sheetData>
-  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
-  <pageSetup paperSize="1" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
-  <headerFooter differentFirst="false" differentOddEven="false">
-    <oddHeader/>
-    <oddFooter/>
-  </headerFooter>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
@@ -809,158 +637,158 @@
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
-        <v>34</v>
+        <v>16</v>
       </c>
       <c r="B1" s="3" t="s">
-        <v>64</v>
+        <v>46</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="1" t="s">
-        <v>37</v>
+        <v>19</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>65</v>
+        <v>47</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B3" s="1" t="s">
-        <v>66</v>
+        <v>48</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B4" s="1" t="s">
-        <v>67</v>
+        <v>49</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B5" s="1" t="s">
-        <v>68</v>
+        <v>50</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B6" s="1" t="s">
-        <v>69</v>
+        <v>51</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B7" s="1" t="s">
-        <v>70</v>
+        <v>52</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B8" s="1" t="s">
-        <v>71</v>
+        <v>53</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B9" s="1" t="s">
-        <v>72</v>
+        <v>54</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B10" s="1" t="s">
-        <v>73</v>
+        <v>55</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B11" s="1" t="s">
-        <v>74</v>
+        <v>56</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B12" s="1" t="s">
-        <v>75</v>
+        <v>57</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B13" s="1" t="s">
-        <v>76</v>
+        <v>58</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B14" s="1" t="s">
-        <v>77</v>
+        <v>59</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B15" s="1" t="s">
-        <v>78</v>
+        <v>60</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B16" s="1" t="s">
-        <v>79</v>
+        <v>61</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B17" s="1" t="s">
-        <v>80</v>
+        <v>62</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B18" s="1" t="s">
-        <v>81</v>
+        <v>63</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B19" s="1" t="s">
-        <v>82</v>
+        <v>64</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B20" s="1" t="s">
-        <v>83</v>
+        <v>65</v>
       </c>
     </row>
     <row r="21" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B21" s="1" t="s">
-        <v>84</v>
+        <v>66</v>
       </c>
     </row>
     <row r="22" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B22" s="1" t="s">
-        <v>85</v>
+        <v>67</v>
       </c>
     </row>
     <row r="23" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B23" s="1" t="s">
-        <v>86</v>
+        <v>68</v>
       </c>
     </row>
     <row r="24" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B24" s="1" t="s">
-        <v>87</v>
+        <v>69</v>
       </c>
     </row>
     <row r="25" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B25" s="1" t="s">
-        <v>88</v>
+        <v>70</v>
       </c>
     </row>
     <row r="26" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B26" s="1" t="s">
-        <v>89</v>
+        <v>71</v>
       </c>
     </row>
     <row r="27" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B27" s="1" t="s">
-        <v>90</v>
+        <v>72</v>
       </c>
     </row>
     <row r="28" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B28" s="1" t="s">
-        <v>91</v>
+        <v>73</v>
       </c>
     </row>
     <row r="29" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B29" s="1" t="s">
-        <v>92</v>
+        <v>74</v>
       </c>
     </row>
     <row r="30" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B30" s="1" t="s">
-        <v>93</v>
+        <v>75</v>
       </c>
     </row>
   </sheetData>
@@ -974,7 +802,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
@@ -996,38 +824,38 @@
   <sheetData>
     <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
-        <v>94</v>
+        <v>76</v>
       </c>
       <c r="B1" s="3" t="s">
-        <v>64</v>
+        <v>46</v>
       </c>
       <c r="C1" s="3" t="s">
-        <v>35</v>
+        <v>17</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>95</v>
+        <v>77</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="1" t="s">
-        <v>35</v>
+        <v>17</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>65</v>
+        <v>47</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>38</v>
+        <v>20</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>96</v>
+        <v>78</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B3" s="1" t="s">
-        <v>66</v>
+        <v>48</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>38</v>
+        <v>20</v>
       </c>
       <c r="D3" s="1" t="n">
         <v>2</v>
@@ -1035,10 +863,10 @@
     </row>
     <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B4" s="1" t="s">
-        <v>67</v>
+        <v>49</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>41</v>
+        <v>23</v>
       </c>
       <c r="D4" s="1" t="n">
         <v>1</v>
@@ -1046,10 +874,10 @@
     </row>
     <row r="5" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B5" s="1" t="s">
-        <v>68</v>
+        <v>50</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>41</v>
+        <v>23</v>
       </c>
       <c r="D5" s="1" t="n">
         <v>2</v>
@@ -1057,10 +885,10 @@
     </row>
     <row r="6" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B6" s="1" t="s">
-        <v>69</v>
+        <v>51</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>41</v>
+        <v>23</v>
       </c>
       <c r="D6" s="1" t="n">
         <v>1</v>
@@ -1068,10 +896,10 @@
     </row>
     <row r="7" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B7" s="1" t="s">
-        <v>70</v>
+        <v>52</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>41</v>
+        <v>23</v>
       </c>
       <c r="D7" s="1" t="n">
         <v>2</v>
@@ -1079,10 +907,10 @@
     </row>
     <row r="8" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B8" s="1" t="s">
-        <v>71</v>
+        <v>53</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>56</v>
+        <v>38</v>
       </c>
       <c r="D8" s="1" t="n">
         <v>1</v>
@@ -1090,10 +918,10 @@
     </row>
     <row r="9" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B9" s="1" t="s">
-        <v>72</v>
+        <v>54</v>
       </c>
       <c r="C9" s="1" t="s">
-        <v>41</v>
+        <v>23</v>
       </c>
       <c r="D9" s="1" t="n">
         <v>2</v>
@@ -1101,10 +929,10 @@
     </row>
     <row r="10" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B10" s="1" t="s">
-        <v>73</v>
+        <v>55</v>
       </c>
       <c r="C10" s="1" t="s">
-        <v>53</v>
+        <v>35</v>
       </c>
       <c r="D10" s="1" t="n">
         <v>1</v>
@@ -1112,10 +940,10 @@
     </row>
     <row r="11" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B11" s="1" t="s">
-        <v>74</v>
+        <v>56</v>
       </c>
       <c r="C11" s="1" t="s">
-        <v>59</v>
+        <v>41</v>
       </c>
       <c r="D11" s="1" t="n">
         <v>2</v>
@@ -1123,10 +951,10 @@
     </row>
     <row r="12" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B12" s="1" t="s">
-        <v>75</v>
+        <v>57</v>
       </c>
       <c r="C12" s="1" t="s">
-        <v>47</v>
+        <v>29</v>
       </c>
       <c r="D12" s="1" t="n">
         <v>1</v>
@@ -1134,10 +962,10 @@
     </row>
     <row r="13" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B13" s="1" t="s">
-        <v>76</v>
+        <v>58</v>
       </c>
       <c r="C13" s="1" t="s">
-        <v>47</v>
+        <v>29</v>
       </c>
       <c r="D13" s="1" t="n">
         <v>2</v>
@@ -1145,10 +973,10 @@
     </row>
     <row r="14" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B14" s="1" t="s">
-        <v>77</v>
+        <v>59</v>
       </c>
       <c r="C14" s="1" t="s">
-        <v>59</v>
+        <v>41</v>
       </c>
       <c r="D14" s="1" t="n">
         <v>1</v>
@@ -1156,10 +984,10 @@
     </row>
     <row r="15" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B15" s="1" t="s">
-        <v>78</v>
+        <v>60</v>
       </c>
       <c r="C15" s="1" t="s">
-        <v>56</v>
+        <v>38</v>
       </c>
       <c r="D15" s="1" t="n">
         <v>2</v>
@@ -1167,10 +995,10 @@
     </row>
     <row r="16" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B16" s="1" t="s">
-        <v>79</v>
+        <v>61</v>
       </c>
       <c r="C16" s="1" t="s">
-        <v>41</v>
+        <v>23</v>
       </c>
       <c r="D16" s="1" t="n">
         <v>1</v>
@@ -1178,10 +1006,10 @@
     </row>
     <row r="17" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B17" s="1" t="s">
-        <v>80</v>
+        <v>62</v>
       </c>
       <c r="C17" s="1" t="s">
-        <v>44</v>
+        <v>26</v>
       </c>
       <c r="D17" s="1" t="n">
         <v>2</v>
@@ -1189,10 +1017,10 @@
     </row>
     <row r="18" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B18" s="1" t="s">
-        <v>81</v>
+        <v>63</v>
       </c>
       <c r="C18" s="1" t="s">
-        <v>53</v>
+        <v>35</v>
       </c>
       <c r="D18" s="1" t="n">
         <v>1</v>
@@ -1200,10 +1028,10 @@
     </row>
     <row r="19" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B19" s="1" t="s">
-        <v>82</v>
+        <v>64</v>
       </c>
       <c r="C19" s="1" t="s">
-        <v>59</v>
+        <v>41</v>
       </c>
       <c r="D19" s="1" t="n">
         <v>2</v>
@@ -1211,10 +1039,10 @@
     </row>
     <row r="20" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B20" s="1" t="s">
-        <v>83</v>
+        <v>65</v>
       </c>
       <c r="C20" s="1" t="s">
-        <v>44</v>
+        <v>26</v>
       </c>
       <c r="D20" s="1" t="n">
         <v>1</v>
@@ -1222,10 +1050,10 @@
     </row>
     <row r="21" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B21" s="1" t="s">
-        <v>84</v>
+        <v>66</v>
       </c>
       <c r="C21" s="1" t="s">
-        <v>44</v>
+        <v>26</v>
       </c>
       <c r="D21" s="1" t="n">
         <v>2</v>
@@ -1233,10 +1061,10 @@
     </row>
     <row r="22" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B22" s="1" t="s">
-        <v>85</v>
+        <v>67</v>
       </c>
       <c r="C22" s="1" t="s">
-        <v>44</v>
+        <v>26</v>
       </c>
       <c r="D22" s="1" t="n">
         <v>1</v>
@@ -1244,10 +1072,10 @@
     </row>
     <row r="23" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B23" s="1" t="s">
-        <v>86</v>
+        <v>68</v>
       </c>
       <c r="C23" s="1" t="s">
-        <v>50</v>
+        <v>32</v>
       </c>
       <c r="D23" s="1" t="n">
         <v>2</v>
@@ -1255,10 +1083,10 @@
     </row>
     <row r="24" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B24" s="1" t="s">
-        <v>87</v>
+        <v>69</v>
       </c>
       <c r="C24" s="1" t="s">
-        <v>50</v>
+        <v>32</v>
       </c>
       <c r="D24" s="1" t="n">
         <v>1</v>
@@ -1266,10 +1094,10 @@
     </row>
     <row r="25" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B25" s="1" t="s">
-        <v>88</v>
+        <v>70</v>
       </c>
       <c r="C25" s="1" t="s">
-        <v>38</v>
+        <v>20</v>
       </c>
       <c r="D25" s="1" t="n">
         <v>2</v>
@@ -1277,10 +1105,10 @@
     </row>
     <row r="26" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B26" s="1" t="s">
-        <v>89</v>
+        <v>71</v>
       </c>
       <c r="C26" s="1" t="s">
-        <v>44</v>
+        <v>26</v>
       </c>
       <c r="D26" s="1" t="n">
         <v>1</v>
@@ -1288,10 +1116,10 @@
     </row>
     <row r="27" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B27" s="1" t="s">
-        <v>90</v>
+        <v>72</v>
       </c>
       <c r="C27" s="1" t="s">
-        <v>44</v>
+        <v>26</v>
       </c>
       <c r="D27" s="1" t="n">
         <v>2</v>
@@ -1299,10 +1127,10 @@
     </row>
     <row r="28" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B28" s="1" t="s">
-        <v>91</v>
+        <v>73</v>
       </c>
       <c r="C28" s="1" t="s">
-        <v>44</v>
+        <v>26</v>
       </c>
       <c r="D28" s="1" t="n">
         <v>1</v>
@@ -1310,10 +1138,10 @@
     </row>
     <row r="29" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B29" s="1" t="s">
-        <v>92</v>
+        <v>74</v>
       </c>
       <c r="C29" s="1" t="s">
-        <v>56</v>
+        <v>38</v>
       </c>
       <c r="D29" s="1" t="n">
         <v>2</v>
@@ -1321,10 +1149,10 @@
     </row>
     <row r="30" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B30" s="1" t="s">
-        <v>93</v>
+        <v>75</v>
       </c>
       <c r="C30" s="1" t="s">
-        <v>53</v>
+        <v>35</v>
       </c>
       <c r="D30" s="1" t="n">
         <v>1</v>

</xml_diff>

<commit_message>
Upates to require angle brackets for @base and @prefix values.
</commit_message>
<xml_diff>
--- a/src/test/resources/custom.xlsx
+++ b/src/test/resources/custom.xlsx
@@ -22,45 +22,27 @@
     <t>Metadata</t>
   </si>
   <si>
-    <t>http://seman.tc/data/northwind</t>
-  </si>
-  <si>
-    <t>http://seman.tc/models/northwind#</t>
-  </si>
-  <si>
     <t>@prefix</t>
   </si>
   <si>
     <t>schema:</t>
   </si>
   <si>
-    <t>http://schema.org/</t>
-  </si>
-  <si>
     <t>foaf:</t>
   </si>
   <si>
-    <t>http://xmlns.com/foaf/0.1/</t>
-  </si>
-  <si>
     <t>northwind:</t>
   </si>
   <si>
     <t>dct:</t>
   </si>
   <si>
-    <t>http://purl.org/dc/terms/</t>
-  </si>
-  <si>
     <t>schema:subject</t>
   </si>
   <si>
     <t>rdfs:label</t>
   </si>
   <si>
-    <t>http://junk/just-for-fun</t>
-  </si>
-  <si>
     <t>Node</t>
   </si>
   <si>
@@ -254,6 +236,24 @@
   </si>
   <si>
     <t>:schema</t>
+  </si>
+  <si>
+    <t>&lt;http://junk/just-for-fun&gt;</t>
+  </si>
+  <si>
+    <t>&lt;http://seman.tc/data/northwind&gt;</t>
+  </si>
+  <si>
+    <t>&lt;http://seman.tc/models/northwind#&gt;</t>
+  </si>
+  <si>
+    <t>&lt;http://schema.org/&gt;</t>
+  </si>
+  <si>
+    <t>&lt;http://xmlns.com/foaf/0.1/&gt;</t>
+  </si>
+  <si>
+    <t>&lt;http://purl.org/dc/terms/&gt;</t>
   </si>
 </sst>
 </file>
@@ -600,7 +600,7 @@
   <dimension ref="A1:D7"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B1" sqref="B1:C2"/>
+      <selection activeCell="D7" sqref="D7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -608,7 +608,7 @@
     <col min="1" max="1" width="9"/>
     <col min="2" max="2" width="19.5703125"/>
     <col min="3" max="3" width="10.28515625"/>
-    <col min="4" max="4" width="31.28515625"/>
+    <col min="4" max="4" width="36.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.25">
@@ -616,85 +616,85 @@
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>77</v>
+        <v>71</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>1</v>
+        <v>74</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" s="1"/>
       <c r="B2" s="1" t="s">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>78</v>
+        <v>72</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>2</v>
+        <v>75</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" s="1"/>
       <c r="B3" s="1" t="s">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="D3" s="1" t="s">
-        <v>5</v>
+        <v>76</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" s="1"/>
       <c r="B4" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C4" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="C4" s="2" t="s">
-        <v>6</v>
-      </c>
       <c r="D4" s="1" t="s">
-        <v>7</v>
+        <v>77</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" s="1"/>
       <c r="B5" s="1" t="s">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="C5" s="2" t="s">
-        <v>8</v>
+        <v>4</v>
       </c>
       <c r="D5" s="1" t="s">
-        <v>2</v>
+        <v>75</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6" s="1"/>
       <c r="B6" s="1" t="s">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="C6" s="2" t="s">
-        <v>9</v>
+        <v>5</v>
       </c>
       <c r="D6" s="1" t="s">
-        <v>10</v>
+        <v>78</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A7" s="1"/>
       <c r="B7" s="1" t="s">
-        <v>11</v>
+        <v>6</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>12</v>
+        <v>7</v>
       </c>
       <c r="D7" s="1" t="s">
-        <v>13</v>
+        <v>73</v>
       </c>
     </row>
   </sheetData>
@@ -727,115 +727,115 @@
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
-        <v>14</v>
+        <v>8</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>15</v>
+        <v>9</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>16</v>
+        <v>10</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>12</v>
+        <v>7</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
-        <v>17</v>
+        <v>11</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>18</v>
+        <v>12</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>19</v>
+        <v>13</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>20</v>
+        <v>14</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B3" s="1" t="s">
-        <v>21</v>
+        <v>15</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>22</v>
+        <v>16</v>
       </c>
       <c r="D3" s="1" t="s">
-        <v>23</v>
+        <v>17</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B4" s="1" t="s">
-        <v>24</v>
+        <v>18</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>25</v>
+        <v>19</v>
       </c>
       <c r="D4" s="1" t="s">
-        <v>26</v>
+        <v>20</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B5" s="1" t="s">
-        <v>27</v>
+        <v>21</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>28</v>
+        <v>22</v>
       </c>
       <c r="D5" s="1" t="s">
-        <v>29</v>
+        <v>23</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B6" s="1" t="s">
-        <v>30</v>
+        <v>24</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>31</v>
+        <v>25</v>
       </c>
       <c r="D6" s="1" t="s">
-        <v>32</v>
+        <v>26</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B7" s="1" t="s">
-        <v>33</v>
+        <v>27</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>34</v>
+        <v>28</v>
       </c>
       <c r="D7" s="1" t="s">
-        <v>35</v>
+        <v>29</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B8" s="1" t="s">
-        <v>36</v>
+        <v>30</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>37</v>
+        <v>31</v>
       </c>
       <c r="D8" s="1" t="s">
-        <v>38</v>
+        <v>32</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B9" s="1" t="s">
-        <v>39</v>
+        <v>33</v>
       </c>
       <c r="C9" s="1" t="s">
-        <v>40</v>
+        <v>34</v>
       </c>
       <c r="D9" s="1" t="s">
-        <v>41</v>
+        <v>35</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B10" s="1" t="s">
-        <v>42</v>
+        <v>36</v>
       </c>
       <c r="C10" s="1" t="s">
-        <v>43</v>
+        <v>37</v>
       </c>
     </row>
   </sheetData>
@@ -861,158 +861,158 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
-        <v>14</v>
+        <v>8</v>
       </c>
       <c r="B1" s="3" t="s">
-        <v>44</v>
+        <v>38</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
-        <v>17</v>
+        <v>11</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>45</v>
+        <v>39</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B3" s="1" t="s">
-        <v>46</v>
+        <v>40</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B4" s="1" t="s">
-        <v>47</v>
+        <v>41</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B5" s="1" t="s">
-        <v>48</v>
+        <v>42</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B6" s="1" t="s">
-        <v>49</v>
+        <v>43</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B7" s="1" t="s">
-        <v>50</v>
+        <v>44</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B8" s="1" t="s">
-        <v>51</v>
+        <v>45</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B9" s="1" t="s">
-        <v>52</v>
+        <v>46</v>
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B10" s="1" t="s">
-        <v>53</v>
+        <v>47</v>
       </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B11" s="1" t="s">
-        <v>54</v>
+        <v>48</v>
       </c>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B12" s="1" t="s">
-        <v>55</v>
+        <v>49</v>
       </c>
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B13" s="1" t="s">
-        <v>56</v>
+        <v>50</v>
       </c>
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B14" s="1" t="s">
-        <v>57</v>
+        <v>51</v>
       </c>
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B15" s="1" t="s">
-        <v>58</v>
+        <v>52</v>
       </c>
     </row>
     <row r="16" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B16" s="1" t="s">
-        <v>59</v>
+        <v>53</v>
       </c>
     </row>
     <row r="17" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B17" s="1" t="s">
-        <v>60</v>
+        <v>54</v>
       </c>
     </row>
     <row r="18" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B18" s="1" t="s">
-        <v>61</v>
+        <v>55</v>
       </c>
     </row>
     <row r="19" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B19" s="1" t="s">
-        <v>62</v>
+        <v>56</v>
       </c>
     </row>
     <row r="20" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B20" s="1" t="s">
-        <v>63</v>
+        <v>57</v>
       </c>
     </row>
     <row r="21" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B21" s="1" t="s">
-        <v>64</v>
+        <v>58</v>
       </c>
     </row>
     <row r="22" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B22" s="1" t="s">
-        <v>65</v>
+        <v>59</v>
       </c>
     </row>
     <row r="23" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B23" s="1" t="s">
-        <v>66</v>
+        <v>60</v>
       </c>
     </row>
     <row r="24" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B24" s="1" t="s">
-        <v>67</v>
+        <v>61</v>
       </c>
     </row>
     <row r="25" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B25" s="1" t="s">
-        <v>68</v>
+        <v>62</v>
       </c>
     </row>
     <row r="26" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B26" s="1" t="s">
-        <v>69</v>
+        <v>63</v>
       </c>
     </row>
     <row r="27" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B27" s="1" t="s">
-        <v>70</v>
+        <v>64</v>
       </c>
     </row>
     <row r="28" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B28" s="1" t="s">
-        <v>71</v>
+        <v>65</v>
       </c>
     </row>
     <row r="29" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B29" s="1" t="s">
-        <v>72</v>
+        <v>66</v>
       </c>
     </row>
     <row r="30" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B30" s="1" t="s">
-        <v>73</v>
+        <v>67</v>
       </c>
     </row>
   </sheetData>
@@ -1044,38 +1044,38 @@
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
-        <v>74</v>
+        <v>68</v>
       </c>
       <c r="B1" s="3" t="s">
-        <v>44</v>
+        <v>38</v>
       </c>
       <c r="C1" s="3" t="s">
-        <v>15</v>
+        <v>9</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>75</v>
+        <v>69</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
-        <v>15</v>
+        <v>9</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>45</v>
+        <v>39</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>18</v>
+        <v>12</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>76</v>
+        <v>70</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B3" s="1" t="s">
-        <v>46</v>
+        <v>40</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>18</v>
+        <v>12</v>
       </c>
       <c r="D3" s="1">
         <v>2</v>
@@ -1083,10 +1083,10 @@
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B4" s="1" t="s">
-        <v>47</v>
+        <v>41</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>21</v>
+        <v>15</v>
       </c>
       <c r="D4" s="1">
         <v>1</v>
@@ -1094,10 +1094,10 @@
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B5" s="1" t="s">
-        <v>48</v>
+        <v>42</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>21</v>
+        <v>15</v>
       </c>
       <c r="D5" s="1">
         <v>2</v>
@@ -1105,10 +1105,10 @@
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B6" s="1" t="s">
-        <v>49</v>
+        <v>43</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>21</v>
+        <v>15</v>
       </c>
       <c r="D6" s="1">
         <v>1</v>
@@ -1116,10 +1116,10 @@
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B7" s="1" t="s">
-        <v>50</v>
+        <v>44</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>21</v>
+        <v>15</v>
       </c>
       <c r="D7" s="1">
         <v>2</v>
@@ -1127,10 +1127,10 @@
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B8" s="1" t="s">
-        <v>51</v>
+        <v>45</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>36</v>
+        <v>30</v>
       </c>
       <c r="D8" s="1">
         <v>1</v>
@@ -1138,10 +1138,10 @@
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B9" s="1" t="s">
-        <v>52</v>
+        <v>46</v>
       </c>
       <c r="C9" s="1" t="s">
-        <v>21</v>
+        <v>15</v>
       </c>
       <c r="D9" s="1">
         <v>2</v>
@@ -1149,10 +1149,10 @@
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B10" s="1" t="s">
-        <v>53</v>
+        <v>47</v>
       </c>
       <c r="C10" s="1" t="s">
-        <v>33</v>
+        <v>27</v>
       </c>
       <c r="D10" s="1">
         <v>1</v>
@@ -1160,10 +1160,10 @@
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B11" s="1" t="s">
-        <v>54</v>
+        <v>48</v>
       </c>
       <c r="C11" s="1" t="s">
-        <v>39</v>
+        <v>33</v>
       </c>
       <c r="D11" s="1">
         <v>2</v>
@@ -1171,10 +1171,10 @@
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B12" s="1" t="s">
-        <v>55</v>
+        <v>49</v>
       </c>
       <c r="C12" s="1" t="s">
-        <v>27</v>
+        <v>21</v>
       </c>
       <c r="D12" s="1">
         <v>1</v>
@@ -1182,10 +1182,10 @@
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B13" s="1" t="s">
-        <v>56</v>
+        <v>50</v>
       </c>
       <c r="C13" s="1" t="s">
-        <v>27</v>
+        <v>21</v>
       </c>
       <c r="D13" s="1">
         <v>2</v>
@@ -1193,10 +1193,10 @@
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B14" s="1" t="s">
-        <v>57</v>
+        <v>51</v>
       </c>
       <c r="C14" s="1" t="s">
-        <v>39</v>
+        <v>33</v>
       </c>
       <c r="D14" s="1">
         <v>1</v>
@@ -1204,10 +1204,10 @@
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B15" s="1" t="s">
-        <v>58</v>
+        <v>52</v>
       </c>
       <c r="C15" s="1" t="s">
-        <v>36</v>
+        <v>30</v>
       </c>
       <c r="D15" s="1">
         <v>2</v>
@@ -1215,10 +1215,10 @@
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B16" s="1" t="s">
-        <v>59</v>
+        <v>53</v>
       </c>
       <c r="C16" s="1" t="s">
-        <v>21</v>
+        <v>15</v>
       </c>
       <c r="D16" s="1">
         <v>1</v>
@@ -1226,10 +1226,10 @@
     </row>
     <row r="17" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B17" s="1" t="s">
-        <v>60</v>
+        <v>54</v>
       </c>
       <c r="C17" s="1" t="s">
-        <v>24</v>
+        <v>18</v>
       </c>
       <c r="D17" s="1">
         <v>2</v>
@@ -1237,10 +1237,10 @@
     </row>
     <row r="18" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B18" s="1" t="s">
-        <v>61</v>
+        <v>55</v>
       </c>
       <c r="C18" s="1" t="s">
-        <v>33</v>
+        <v>27</v>
       </c>
       <c r="D18" s="1">
         <v>1</v>
@@ -1248,10 +1248,10 @@
     </row>
     <row r="19" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B19" s="1" t="s">
-        <v>62</v>
+        <v>56</v>
       </c>
       <c r="C19" s="1" t="s">
-        <v>39</v>
+        <v>33</v>
       </c>
       <c r="D19" s="1">
         <v>2</v>
@@ -1259,10 +1259,10 @@
     </row>
     <row r="20" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B20" s="1" t="s">
-        <v>63</v>
+        <v>57</v>
       </c>
       <c r="C20" s="1" t="s">
-        <v>24</v>
+        <v>18</v>
       </c>
       <c r="D20" s="1">
         <v>1</v>
@@ -1270,10 +1270,10 @@
     </row>
     <row r="21" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B21" s="1" t="s">
-        <v>64</v>
+        <v>58</v>
       </c>
       <c r="C21" s="1" t="s">
-        <v>24</v>
+        <v>18</v>
       </c>
       <c r="D21" s="1">
         <v>2</v>
@@ -1281,10 +1281,10 @@
     </row>
     <row r="22" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B22" s="1" t="s">
-        <v>65</v>
+        <v>59</v>
       </c>
       <c r="C22" s="1" t="s">
-        <v>24</v>
+        <v>18</v>
       </c>
       <c r="D22" s="1">
         <v>1</v>
@@ -1292,10 +1292,10 @@
     </row>
     <row r="23" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B23" s="1" t="s">
-        <v>66</v>
+        <v>60</v>
       </c>
       <c r="C23" s="1" t="s">
-        <v>30</v>
+        <v>24</v>
       </c>
       <c r="D23" s="1">
         <v>2</v>
@@ -1303,10 +1303,10 @@
     </row>
     <row r="24" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B24" s="1" t="s">
-        <v>67</v>
+        <v>61</v>
       </c>
       <c r="C24" s="1" t="s">
-        <v>30</v>
+        <v>24</v>
       </c>
       <c r="D24" s="1">
         <v>1</v>
@@ -1314,10 +1314,10 @@
     </row>
     <row r="25" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B25" s="1" t="s">
-        <v>68</v>
+        <v>62</v>
       </c>
       <c r="C25" s="1" t="s">
-        <v>18</v>
+        <v>12</v>
       </c>
       <c r="D25" s="1">
         <v>2</v>
@@ -1325,10 +1325,10 @@
     </row>
     <row r="26" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B26" s="1" t="s">
-        <v>69</v>
+        <v>63</v>
       </c>
       <c r="C26" s="1" t="s">
-        <v>24</v>
+        <v>18</v>
       </c>
       <c r="D26" s="1">
         <v>1</v>
@@ -1336,10 +1336,10 @@
     </row>
     <row r="27" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B27" s="1" t="s">
-        <v>70</v>
+        <v>64</v>
       </c>
       <c r="C27" s="1" t="s">
-        <v>24</v>
+        <v>18</v>
       </c>
       <c r="D27" s="1">
         <v>2</v>
@@ -1347,10 +1347,10 @@
     </row>
     <row r="28" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B28" s="1" t="s">
-        <v>71</v>
+        <v>65</v>
       </c>
       <c r="C28" s="1" t="s">
-        <v>24</v>
+        <v>18</v>
       </c>
       <c r="D28" s="1">
         <v>1</v>
@@ -1358,10 +1358,10 @@
     </row>
     <row r="29" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B29" s="1" t="s">
-        <v>72</v>
+        <v>66</v>
       </c>
       <c r="C29" s="1" t="s">
-        <v>36</v>
+        <v>30</v>
       </c>
       <c r="D29" s="1">
         <v>2</v>
@@ -1369,10 +1369,10 @@
     </row>
     <row r="30" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B30" s="1" t="s">
-        <v>73</v>
+        <v>67</v>
       </c>
       <c r="C30" s="1" t="s">
-        <v>33</v>
+        <v>27</v>
       </c>
       <c r="D30" s="1">
         <v>1</v>

</xml_diff>